<commit_message>
Fixes on single board
</commit_message>
<xml_diff>
--- a/Boards/Single_board/BOM/JLC_Top.xlsx
+++ b/Boards/Single_board/BOM/JLC_Top.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Comment</t>
   </si>
@@ -106,6 +106,9 @@
     <t>D=3mm THT White led</t>
   </si>
   <si>
+    <t>C2895458</t>
+  </si>
+  <si>
     <t>R2,R31,R32,R30,R3,R34,R29,R22,R26,R16,R19,R12,R9,R14,R13,R27,R25,R23,R17,R24,R21,R15,R20,R10,R18,R11</t>
   </si>
   <si>
@@ -142,7 +145,7 @@
     <t>1206 Orange LED</t>
   </si>
   <si>
-    <t>C264537</t>
+    <t>C2764895</t>
   </si>
   <si>
     <t>Keyboard switches</t>
@@ -154,6 +157,9 @@
     <t>MX</t>
   </si>
   <si>
+    <t>C5120587</t>
+  </si>
+  <si>
     <t>R42,R37,R40,R39,R38,R35,R36,R41,R43</t>
   </si>
   <si>
@@ -187,10 +193,10 @@
     <t>D34</t>
   </si>
   <si>
-    <t>SD101AWS Diode</t>
-  </si>
-  <si>
-    <t>C2992004</t>
+    <t>MBR0520LT1G</t>
+  </si>
+  <si>
+    <t>C23848</t>
   </si>
   <si>
     <t>U1</t>
@@ -921,7 +927,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -933,6 +939,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1470,7 +1479,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1520,7 +1529,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1530,207 +1539,213 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="B14" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="B15" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="2:2">

</xml_diff>

<commit_message>
Update white leds to comply with JLC's request
</commit_message>
<xml_diff>
--- a/Boards/Single_board/BOM/JLC_Top.xlsx
+++ b/Boards/Single_board/BOM/JLC_Top.xlsx
@@ -136,7 +136,7 @@
     <t>1206 White LED</t>
   </si>
   <si>
-    <t>C375565</t>
+    <t>C412285</t>
   </si>
   <si>
     <t>D33,D29,D28,D27,D26,D30,D31,D25,D32</t>
@@ -1479,7 +1479,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>

</xml_diff>